<commit_message>
combined JW books and Website
</commit_message>
<xml_diff>
--- a/Medical Data.xlsx
+++ b/Medical Data.xlsx
@@ -470,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B3" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>